<commit_message>
spr 20240227 add ToneBurst
</commit_message>
<xml_diff>
--- a/ThreeScalesStatistic/ThreeScales_ClickTrain_Config.xlsx
+++ b/ThreeScalesStatistic/ThreeScales_ClickTrain_Config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D4A851-BE32-4637-809B-683BFE576AD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641A5C81-52EF-4522-9D45-78110599B588}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1332" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1335" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="98">
   <si>
     <t>Amp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,6 +403,14 @@
   </si>
   <si>
     <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024/2/21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4;4,8;4,16;4,32;4,64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -793,56 +801,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP10"/>
+  <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="14.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.125" style="12" customWidth="1"/>
     <col min="5" max="5" width="9" style="11"/>
-    <col min="6" max="6" width="44.5546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="12" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" style="12" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" style="12" customWidth="1"/>
-    <col min="12" max="13" width="15.88671875" style="12" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.33203125" style="16" customWidth="1"/>
-    <col min="16" max="16" width="16.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.77734375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="27.33203125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="32.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="44.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="19.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="13.875" style="12" customWidth="1"/>
+    <col min="10" max="10" width="12.75" style="13" customWidth="1"/>
+    <col min="11" max="11" width="8.125" style="12" customWidth="1"/>
+    <col min="12" max="13" width="15.875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="20.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.375" style="16" customWidth="1"/>
+    <col min="16" max="16" width="16.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.75" style="13" customWidth="1"/>
+    <col min="18" max="18" width="27.375" style="13" customWidth="1"/>
+    <col min="19" max="19" width="32.625" style="13" customWidth="1"/>
     <col min="20" max="22" width="24" style="13" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" style="13" customWidth="1"/>
-    <col min="24" max="24" width="23.33203125" style="13" customWidth="1"/>
-    <col min="25" max="26" width="12.44140625" style="13" customWidth="1"/>
-    <col min="27" max="27" width="14.44140625" style="13" customWidth="1"/>
+    <col min="23" max="23" width="12.5" style="13" customWidth="1"/>
+    <col min="24" max="24" width="23.375" style="13" customWidth="1"/>
+    <col min="25" max="26" width="12.5" style="13" customWidth="1"/>
+    <col min="27" max="27" width="14.5" style="13" customWidth="1"/>
     <col min="28" max="28" width="14" style="13" customWidth="1"/>
-    <col min="29" max="29" width="70.88671875" style="17" customWidth="1"/>
+    <col min="29" max="29" width="70.875" style="17" customWidth="1"/>
     <col min="30" max="31" width="18" style="17" customWidth="1"/>
-    <col min="32" max="32" width="19.21875" style="13" customWidth="1"/>
-    <col min="33" max="33" width="17.109375" style="13" customWidth="1"/>
-    <col min="34" max="34" width="16.109375" style="13" customWidth="1"/>
-    <col min="35" max="35" width="21.109375" style="13" customWidth="1"/>
+    <col min="32" max="32" width="19.25" style="13" customWidth="1"/>
+    <col min="33" max="33" width="17.125" style="13" customWidth="1"/>
+    <col min="34" max="34" width="16.125" style="13" customWidth="1"/>
+    <col min="35" max="35" width="21.125" style="13" customWidth="1"/>
     <col min="36" max="36" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.44140625" style="11" customWidth="1"/>
-    <col min="40" max="40" width="11.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.109375" style="11" customWidth="1"/>
-    <col min="42" max="42" width="29.6640625" style="18" customWidth="1"/>
+    <col min="37" max="37" width="8.125" style="18" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5" style="11" customWidth="1"/>
+    <col min="40" max="40" width="11.875" style="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.125" style="11" customWidth="1"/>
+    <col min="42" max="42" width="29.625" style="18" customWidth="1"/>
     <col min="43" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -970,7 +978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:42" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1098,7 +1106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>101</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>102</v>
       </c>
@@ -1258,24 +1266,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
-        <v>103</v>
+        <v>102.1</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C5" s="14">
         <v>97656</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>55</v>
@@ -1303,16 +1311,16 @@
         <v>65</v>
       </c>
       <c r="S5" s="13" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="T5" s="13" t="s">
         <v>88</v>
       </c>
       <c r="U5" s="13" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="W5" s="8" t="s">
         <v>27</v>
@@ -1335,12 +1343,12 @@
         <v>14</v>
       </c>
       <c r="AP5" s="18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>53</v>
@@ -1355,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>55</v>
@@ -1377,13 +1385,13 @@
         <v>64</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="R6" s="13" t="s">
         <v>65</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="T6" s="13" t="s">
         <v>88</v>
@@ -1418,138 +1426,130 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:42" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>103.1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="14">
+        <v>97656</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="11">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="16">
+        <v>2000</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="T7" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="V7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP7" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="25"/>
-      <c r="AD7" s="25"/>
-      <c r="AE7" s="25"/>
-      <c r="AF7" s="20"/>
-      <c r="AG7" s="20"/>
-      <c r="AH7" s="20"/>
-      <c r="AI7" s="20"/>
-      <c r="AK7" s="26"/>
-      <c r="AL7" s="26"/>
-      <c r="AP7" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="25"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
+      <c r="AP8" s="26"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
         <v>201</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="14">
-        <v>97656</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="11">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="12">
-        <v>1.8</v>
-      </c>
-      <c r="I8" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="K8" s="12">
-        <v>4</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="O8" s="16">
-        <v>2000</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="S8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="T8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="U8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="V8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="W8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP8" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>202</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>53</v>
@@ -1558,13 +1558,13 @@
         <v>97656</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="11">
         <v>1</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>55</v>
@@ -1576,7 +1576,7 @@
         <v>0.5</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K9" s="12">
         <v>4</v>
@@ -1597,13 +1597,13 @@
         <v>35</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="T9" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U9" s="13" t="s">
         <v>27</v>
@@ -1629,15 +1629,15 @@
         <v>20</v>
       </c>
       <c r="AN9" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AP9" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>53</v>
@@ -1646,13 +1646,13 @@
         <v>97656</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E10" s="11">
         <v>1</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>55</v>
@@ -1688,16 +1688,16 @@
         <v>65</v>
       </c>
       <c r="S10" s="13" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="T10" s="13" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="U10" s="13" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="V10" s="13" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="W10" s="8" t="s">
         <v>27</v>
@@ -1720,6 +1720,94 @@
         <v>14</v>
       </c>
       <c r="AP10" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>203</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="14">
+        <v>97656</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="12">
+        <v>4</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O11" s="16">
+        <v>2000</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="S11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="T11" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="V11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA11" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP11" s="18" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1738,44 +1826,44 @@
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="10">
         <v>402.44</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>402.44099999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>403.44</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>404.44</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>404.44099999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>405.44</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>406.44</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>407.44</v>
       </c>

</xml_diff>